<commit_message>
modified test scenarios and test case
</commit_message>
<xml_diff>
--- a/src/main/resources/TestCase Template.xlsx
+++ b/src/main/resources/TestCase Template.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\AutomationTest\GiaoTrinh\Bai tap nhom\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DOCUMENTS\N3 - DOCUMENTS\SOFTWARE TESTING\Software-Testing\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26BF6DBF-2F7C-4E6D-827D-1D906FED0D2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Logout" sheetId="3" r:id="rId2"/>
+    <sheet name="New Customer" sheetId="5" r:id="rId3"/>
+    <sheet name="New Account" sheetId="6" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Login!$A$1:$H$29</definedName>
@@ -29,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="129">
   <si>
     <t>Test Steps</t>
   </si>
@@ -89,12 +92,385 @@
   <si>
     <t>author?</t>
   </si>
+  <si>
+    <t>TC002</t>
+  </si>
+  <si>
+    <t>TC003</t>
+  </si>
+  <si>
+    <t>TC004</t>
+  </si>
+  <si>
+    <t>TC005</t>
+  </si>
+  <si>
+    <t>TC006</t>
+  </si>
+  <si>
+    <t>TC007</t>
+  </si>
+  <si>
+    <t>TC008</t>
+  </si>
+  <si>
+    <t>TC009</t>
+  </si>
+  <si>
+    <t>TC010</t>
+  </si>
+  <si>
+    <t>TC011</t>
+  </si>
+  <si>
+    <t>TC012</t>
+  </si>
+  <si>
+    <t>TC013</t>
+  </si>
+  <si>
+    <t>TC014</t>
+  </si>
+  <si>
+    <t>TC015</t>
+  </si>
+  <si>
+    <t>TC016</t>
+  </si>
+  <si>
+    <t>TC017</t>
+  </si>
+  <si>
+    <t>TC018</t>
+  </si>
+  <si>
+    <t>TC019</t>
+  </si>
+  <si>
+    <t>TC020</t>
+  </si>
+  <si>
+    <t>TC021</t>
+  </si>
+  <si>
+    <t>TC022</t>
+  </si>
+  <si>
+    <t>1) Do not enter a value in NAME Field
+2) Press TAB and move to next Field</t>
+  </si>
+  <si>
+    <t>1) Enter numeric value in NAME Field</t>
+  </si>
+  <si>
+    <t>1) Enter Special Character In NAME Field</t>
+  </si>
+  <si>
+    <t>1) Enter First character Blank space</t>
+  </si>
+  <si>
+    <t>1234
+name123</t>
+  </si>
+  <si>
+    <t>name!@#
+!@#</t>
+  </si>
+  <si>
+    <t>An error message "Customer name must not be blank" must shown</t>
+  </si>
+  <si>
+    <t>An error message "Numbers are not allowed" must be shown</t>
+  </si>
+  <si>
+    <t>An error message "Special characters are not allowed" must be shown</t>
+  </si>
+  <si>
+    <t>An error message "First character cannot be space" must be shown</t>
+  </si>
+  <si>
+    <t>Trung Kỳ</t>
+  </si>
+  <si>
+    <t>1) Do not enter a value in ADDRESS Field
+2) Press TAB and move to next Field</t>
+  </si>
+  <si>
+    <t>An error message "ADDRESS cannot be empty" must be shown</t>
+  </si>
+  <si>
+    <t>1) Do not enter a value in CITY Field
+2) Press TAB and move to next Field</t>
+  </si>
+  <si>
+    <t>An error message "City Field must be not blank" must be shown</t>
+  </si>
+  <si>
+    <t>1) Enter numeric value in CITY Field</t>
+  </si>
+  <si>
+    <t>1234
+city123</t>
+  </si>
+  <si>
+    <t>1) Enter Special Character In CITY Field</t>
+  </si>
+  <si>
+    <t>City!@#
+!@#</t>
+  </si>
+  <si>
+    <t>1) Do not enter a value in STATE Field
+2) Press TAB and move to next Field</t>
+  </si>
+  <si>
+    <t>An error message "State must not be blank" must be shown</t>
+  </si>
+  <si>
+    <t>1) Enter numeric value in STATE Field</t>
+  </si>
+  <si>
+    <t>1234
+State123</t>
+  </si>
+  <si>
+    <t>1) Enter Special Character In STATE Field</t>
+  </si>
+  <si>
+    <t>State!@#
+!@#</t>
+  </si>
+  <si>
+    <t>1) Enter character value in PIN Field</t>
+  </si>
+  <si>
+    <t>1234
+1234PIN</t>
+  </si>
+  <si>
+    <t>An error message "Characters are not allowed" must be shown</t>
+  </si>
+  <si>
+    <t>1) Do not enter a value in PIN Field
+2) Press TAB and move to next Field</t>
+  </si>
+  <si>
+    <t>An error message "PIN code must not be blank" must be shown</t>
+  </si>
+  <si>
+    <t>1) Enter More than 6 digit in PIN field
+2) Enter Less Than 6 digit in PIN field</t>
+  </si>
+  <si>
+    <t>12
+123</t>
+  </si>
+  <si>
+    <t>An error message "PIN Code must have 6 Digits" must be shown</t>
+  </si>
+  <si>
+    <t>1) Enter Special Character In PIN Field</t>
+  </si>
+  <si>
+    <t>!@#
+123!@#</t>
+  </si>
+  <si>
+    <t>An error message "PIN cannot have space" must be shown</t>
+  </si>
+  <si>
+    <t>1) Do not enter a value in Telephone Field
+2) Press TAB and move to next Field</t>
+  </si>
+  <si>
+    <t>An error message "Telephone no must not be blank" must be shown</t>
+  </si>
+  <si>
+    <t>1) Enter Blank space in Telephone</t>
+  </si>
+  <si>
+    <t>123 123</t>
+  </si>
+  <si>
+    <t>An error message "Telephone cannot have be space" must be shown</t>
+  </si>
+  <si>
+    <t>1) Enter Special Character In Telephone Field</t>
+  </si>
+  <si>
+    <t>886636!@12
+!@88662682
+88663682!@</t>
+  </si>
+  <si>
+    <t>1) Do not enter a value in Email Field
+2) Press TAB and move to next Field</t>
+  </si>
+  <si>
+    <t>An error message "Email ID must not be blank" must be shown</t>
+  </si>
+  <si>
+    <t>Enter invalid email in Email field</t>
+  </si>
+  <si>
+    <t>guru99@gmail
+guru99
+Guru99@
+guru99@gmail.
+guru99gmail.com</t>
+  </si>
+  <si>
+    <t>An error message "Email-ID is not valid"" must be shown</t>
+  </si>
+  <si>
+    <t>1) Enter Blank space in Email</t>
+  </si>
+  <si>
+    <t>An error message "Email-ID is not valid" must be shown</t>
+  </si>
+  <si>
+    <t>Observe to fields name</t>
+  </si>
+  <si>
+    <t>Field name:
+Customer Name
+Gender
+Date of Birth
+Address
+City
+State
+PIN
+Mobile Number
+E-mail
+Password</t>
+  </si>
+  <si>
+    <t>TC023</t>
+  </si>
+  <si>
+    <t>TC024</t>
+  </si>
+  <si>
+    <t>TC025</t>
+  </si>
+  <si>
+    <t>TC026</t>
+  </si>
+  <si>
+    <t>TC027</t>
+  </si>
+  <si>
+    <t>TC028</t>
+  </si>
+  <si>
+    <t>1) Do not enter a value in Customer id Field
+2) Press TAB and move to next Field</t>
+  </si>
+  <si>
+    <t>An error message "Customer ID must not blank" must be shown</t>
+  </si>
+  <si>
+    <t>1) Enter character value in Customer id Field</t>
+  </si>
+  <si>
+    <t>1234Acc
+Acc123</t>
+  </si>
+  <si>
+    <t>An error message "Customer id must be numeric" must be shown</t>
+  </si>
+  <si>
+    <t>1) Enter Special Character In Customer id Field</t>
+  </si>
+  <si>
+    <t>123!@#
+!@#</t>
+  </si>
+  <si>
+    <t>An error message "Customer id cannot have special character" must be shown</t>
+  </si>
+  <si>
+    <t>1) Customer Id cannot have Blank space
+2) Press Tab</t>
+  </si>
+  <si>
+    <t>123 12</t>
+  </si>
+  <si>
+    <t>An error message "Customer id cannot have blank space" must be shown</t>
+  </si>
+  <si>
+    <t>1) Enter first character space
+2) Press Tab</t>
+  </si>
+  <si>
+    <t>An error message "Customer id cannot have first character space" must be shown</t>
+  </si>
+  <si>
+    <t>1) Do not enter a value in Initial Deposit Field
+2) Press TAB and move to next Field</t>
+  </si>
+  <si>
+    <t>An error message "Initial deposit cannot be empty" must be shown</t>
+  </si>
+  <si>
+    <t>1) Enter character value in Initial Deposit Field</t>
+  </si>
+  <si>
+    <t>An error message "Initial Deposit must be numeric" must be shown</t>
+  </si>
+  <si>
+    <t>1) Enter Special Character In Initial Deposit Field</t>
+  </si>
+  <si>
+    <t>An error message "Initial Deposit cannot have special character" must be shown</t>
+  </si>
+  <si>
+    <t>1) Initial Deposit cannot have Blank space
+2) Press Tab</t>
+  </si>
+  <si>
+    <t>An error message "Initial Deposit cannot have blank space" must be shown</t>
+  </si>
+  <si>
+    <t>An error message "Initial Deposit cannot have first character space" must be shown</t>
+  </si>
+  <si>
+    <t>TC_29</t>
+  </si>
+  <si>
+    <t>TC_30</t>
+  </si>
+  <si>
+    <t>TC_31</t>
+  </si>
+  <si>
+    <t>TC_32</t>
+  </si>
+  <si>
+    <t>TC_33</t>
+  </si>
+  <si>
+    <t>TC_34</t>
+  </si>
+  <si>
+    <t>TC_35</t>
+  </si>
+  <si>
+    <t>TC_36</t>
+  </si>
+  <si>
+    <t>TC_37</t>
+  </si>
+  <si>
+    <t>TC_38</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -115,8 +491,46 @@
       <color rgb="FFFFFFFF"/>
       <name val="Droid Sans"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Droid Sans"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Docs-Nunito"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Docs-Nunito"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Be Vietnam"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
+      <name val="Be Vietnam"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -147,11 +561,97 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFE599"/>
+        <bgColor rgb="FFFFE599"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -160,7 +660,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -191,6 +691,52 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -471,7 +1017,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -2955,21 +3501,21 @@
       <c r="V101" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H29"/>
+  <autoFilter ref="A1:H29" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:V101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:I1"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" customHeight="1"/>
@@ -5445,7 +5991,853 @@
       <c r="V101" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H29"/>
+  <autoFilter ref="A1:H29" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{308B1486-C1F4-4024-AE37-29FF1D0216E6}">
+  <dimension ref="A1:I32"/>
+  <sheetViews>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="39.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="41" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" customWidth="1"/>
+    <col min="5" max="6" width="33.28515625" customWidth="1"/>
+    <col min="7" max="7" width="20" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" customWidth="1"/>
+    <col min="9" max="9" width="22.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="51">
+      <c r="A2" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="25.5">
+      <c r="A3" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="25.5">
+      <c r="A4" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="25.5">
+      <c r="A5" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="51">
+      <c r="A6" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="25.5">
+      <c r="A7" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="51">
+      <c r="A8" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="25.5">
+      <c r="A9" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="25.5">
+      <c r="A10" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="25.5">
+      <c r="A11" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="51">
+      <c r="A12" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I12" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="25.5">
+      <c r="A13" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I13" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="25.5">
+      <c r="A14" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I14" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="25.5">
+      <c r="A15" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I15" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="25.5">
+      <c r="A16" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I16" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="51">
+      <c r="A17" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="H17" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I17" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="51">
+      <c r="A18" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="H18" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I18" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="25.5">
+      <c r="A19" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I19" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="25.5">
+      <c r="A20" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="H20" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I20" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="25.5">
+      <c r="A21" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="H21" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I21" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="51">
+      <c r="A22" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="H22" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I22" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="25.5">
+      <c r="A23" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="H23" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I23" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="25.5">
+      <c r="A24" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="H24" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I24" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="38.25">
+      <c r="A25" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I25" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="51">
+      <c r="A26" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I26" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="63.75">
+      <c r="A27" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="H27" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I27" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="25.5">
+      <c r="A28" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I28" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="140.25">
+      <c r="A29" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="E29" s="15"/>
+      <c r="F29" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="H29" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I29" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="I30" s="18"/>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="I31" s="18"/>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="I32" s="18"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E04F4AFE-68E0-477C-9F5B-1ED363B00243}">
+  <dimension ref="A1:I11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="30.85546875" customWidth="1"/>
+    <col min="4" max="4" width="64" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" customWidth="1"/>
+    <col min="6" max="6" width="44.7109375" customWidth="1"/>
+    <col min="7" max="7" width="49.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="38.25">
+      <c r="A1" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="50.25" thickBot="1">
+      <c r="A2" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="75" thickBot="1">
+      <c r="A3" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="75" thickBot="1">
+      <c r="A4" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="75" thickBot="1">
+      <c r="A5" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="75" thickBot="1">
+      <c r="A6" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="74.25">
+      <c r="A7" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" s="21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="74.25">
+      <c r="A8" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" s="21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="74.25">
+      <c r="A9" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" s="21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="74.25">
+      <c r="A10" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" s="21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="75" thickBot="1">
+      <c r="A11" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11" s="21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Test Scenario and Test Case
</commit_message>
<xml_diff>
--- a/src/main/resources/TestCase Template.xlsx
+++ b/src/main/resources/TestCase Template.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Logout" sheetId="3" r:id="rId2"/>
     <sheet name="Deposit" sheetId="8" r:id="rId3"/>
     <sheet name="Withdrawal" sheetId="9" r:id="rId4"/>
-    <sheet name="NewAccount" sheetId="10" r:id="rId5"/>
-    <sheet name="NewCustomer" sheetId="11" r:id="rId6"/>
+    <sheet name="New Customer" sheetId="10" r:id="rId5"/>
+    <sheet name="New Account" sheetId="11" r:id="rId6"/>
     <sheet name="Customized Statement" sheetId="12" r:id="rId7"/>
     <sheet name="Fund Transfer" sheetId="13" r:id="rId8"/>
   </sheets>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="333">
   <si>
     <t>Test Steps</t>
   </si>
@@ -1154,12 +1154,135 @@
   <si>
     <t>Hoàng Thanh Tùng</t>
   </si>
+  <si>
+    <t>Name cannot be empty</t>
+  </si>
+  <si>
+    <t>Name cannot be numeric</t>
+  </si>
+  <si>
+    <t>Name cannot have special characters</t>
+  </si>
+  <si>
+    <t>Name cannot have first character as blank space</t>
+  </si>
+  <si>
+    <t>Address cannot be empty</t>
+  </si>
+  <si>
+    <t>Address cannot have first blank space</t>
+  </si>
+  <si>
+    <t>City cannot be empty</t>
+  </si>
+  <si>
+    <t>City cannot be numeric</t>
+  </si>
+  <si>
+    <t>City cannot have special
+character</t>
+  </si>
+  <si>
+    <t>City cannot have first blank space</t>
+  </si>
+  <si>
+    <t>State cannot be empty</t>
+  </si>
+  <si>
+    <t>State cannot be numeric</t>
+  </si>
+  <si>
+    <t>State cannot have special
+character</t>
+  </si>
+  <si>
+    <t>State cannot have first blank space</t>
+  </si>
+  <si>
+    <t>PIN must be numeric</t>
+  </si>
+  <si>
+    <t>PIN cannot be empty</t>
+  </si>
+  <si>
+    <t>PIN must have 6 digits</t>
+  </si>
+  <si>
+    <t>PIN cannot have special character</t>
+  </si>
+  <si>
+    <t>PIN cannot have first blank space</t>
+  </si>
+  <si>
+    <t>PIN cannot have blank space</t>
+  </si>
+  <si>
+    <t>Telephone cannot be empty</t>
+  </si>
+  <si>
+    <t>Telephone cannot have first character as blank space</t>
+  </si>
+  <si>
+    <t>Telephone cannot have spaces</t>
+  </si>
+  <si>
+    <t>Telephone cannot have special character</t>
+  </si>
+  <si>
+    <t>Email cannot be empty</t>
+  </si>
+  <si>
+    <t>Email must be in correct format</t>
+  </si>
+  <si>
+    <t>Email cannot have space</t>
+  </si>
+  <si>
+    <t>Check all Fields name (label) are as requirement</t>
+  </si>
+  <si>
+    <t>Customer id cannot be empty</t>
+  </si>
+  <si>
+    <t>Customer id must be numeric</t>
+  </si>
+  <si>
+    <t>Customer id cannot have special character</t>
+  </si>
+  <si>
+    <t>Customer id cannot have blank space</t>
+  </si>
+  <si>
+    <t>First Character cannot be space</t>
+  </si>
+  <si>
+    <t>Cannot be empty</t>
+  </si>
+  <si>
+    <t>Must be numeric</t>
+  </si>
+  <si>
+    <t>Cannot have special character</t>
+  </si>
+  <si>
+    <t>Initial Deposit cannot have blank space</t>
+  </si>
+  <si>
+    <t>New Account Form open
+Manager account is logged
+A customer must be exists.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Customer Form open
+Manager account is logged
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1175,21 +1298,9 @@
       <name val="Droid Sans"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1348,7 +1459,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1374,201 +1485,185 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1857,7 +1952,7 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" customHeight="1"/>
@@ -1917,31 +2012,31 @@
       <c r="V1" s="7"/>
     </row>
     <row r="2" spans="1:22" ht="63">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="27" t="s">
+      <c r="G2" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="27" t="s">
+      <c r="H2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="28" t="s">
+      <c r="I2" s="37" t="s">
         <v>277</v>
       </c>
       <c r="J2" s="3"/>
@@ -1959,31 +2054,31 @@
       <c r="V2" s="3"/>
     </row>
     <row r="3" spans="1:22" ht="63">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="G3" s="27" t="s">
+      <c r="G3" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="H3" s="27" t="s">
+      <c r="H3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="29"/>
+      <c r="I3" s="38"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
@@ -1999,31 +2094,31 @@
       <c r="V3" s="4"/>
     </row>
     <row r="4" spans="1:22" ht="63">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="G4" s="27" t="s">
+      <c r="G4" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="H4" s="27" t="s">
+      <c r="H4" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="29"/>
+      <c r="I4" s="38"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
@@ -2039,31 +2134,31 @@
       <c r="V4" s="4"/>
     </row>
     <row r="5" spans="1:22" ht="47.25">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="E5" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="F5" s="27" t="s">
+      <c r="F5" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="G5" s="27" t="s">
+      <c r="G5" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="H5" s="27" t="s">
+      <c r="H5" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="29"/>
+      <c r="I5" s="38"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
@@ -2079,31 +2174,31 @@
       <c r="V5" s="4"/>
     </row>
     <row r="6" spans="1:22" ht="47.25">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="27" t="s">
+      <c r="D6" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="E6" s="27" t="s">
+      <c r="E6" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="F6" s="27" t="s">
+      <c r="F6" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="G6" s="27" t="s">
+      <c r="G6" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="H6" s="27" t="s">
+      <c r="H6" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="29"/>
+      <c r="I6" s="38"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
@@ -2119,31 +2214,31 @@
       <c r="V6" s="4"/>
     </row>
     <row r="7" spans="1:22" ht="63">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="27" t="s">
+      <c r="D7" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="E7" s="27" t="s">
+      <c r="E7" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="F7" s="27" t="s">
+      <c r="F7" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="G7" s="27" t="s">
+      <c r="G7" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="H7" s="27" t="s">
+      <c r="H7" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="30"/>
+      <c r="I7" s="39"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
@@ -3785,7 +3880,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75"/>
@@ -3802,31 +3897,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="8" customFormat="1" ht="15.75">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="60" t="s">
+      <c r="C1" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="60" t="s">
+      <c r="D1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="60" t="s">
+      <c r="E1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="60" t="s">
+      <c r="F1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="60" t="s">
+      <c r="G1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="60" t="s">
+      <c r="H1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="61" t="s">
+      <c r="I1" s="26" t="s">
         <v>13</v>
       </c>
       <c r="J1" s="7"/>
@@ -3844,27 +3939,27 @@
       <c r="V1" s="7"/>
     </row>
     <row r="2" spans="1:22" ht="47.25">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="C2" s="59" t="s">
+      <c r="C2" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="D2" s="59" t="s">
+      <c r="D2" s="24" t="s">
         <v>126</v>
       </c>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59" t="s">
+      <c r="E2" s="24"/>
+      <c r="F2" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="G2" s="59" t="s">
+      <c r="G2" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="H2" s="59"/>
-      <c r="I2" s="70" t="s">
+      <c r="H2" s="24"/>
+      <c r="I2" s="40" t="s">
         <v>278</v>
       </c>
       <c r="J2" s="3"/>
@@ -3882,31 +3977,31 @@
       <c r="V2" s="3"/>
     </row>
     <row r="3" spans="1:22" ht="31.5">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="D3" s="59" t="s">
+      <c r="D3" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="E3" s="59" t="s">
+      <c r="E3" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="F3" s="59" t="s">
+      <c r="F3" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="G3" s="59" t="s">
+      <c r="G3" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="H3" s="59" t="s">
+      <c r="H3" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="72"/>
+      <c r="I3" s="41"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
@@ -3922,31 +4017,31 @@
       <c r="V3" s="4"/>
     </row>
     <row r="4" spans="1:22" ht="78.75">
-      <c r="A4" s="56" t="s">
+      <c r="A4" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="71" t="s">
+      <c r="B4" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="C4" s="59" t="s">
+      <c r="C4" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="D4" s="59" t="s">
+      <c r="D4" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="E4" s="59" t="s">
+      <c r="E4" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="F4" s="73" t="s">
+      <c r="F4" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="G4" s="73" t="s">
+      <c r="G4" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="H4" s="59" t="s">
+      <c r="H4" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="72"/>
+      <c r="I4" s="41"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
@@ -3962,31 +4057,31 @@
       <c r="V4" s="4"/>
     </row>
     <row r="5" spans="1:22" ht="47.25">
-      <c r="A5" s="56" t="s">
+      <c r="A5" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="B5" s="71" t="s">
+      <c r="B5" s="32" t="s">
         <v>103</v>
       </c>
-      <c r="C5" s="59" t="s">
+      <c r="C5" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="D5" s="59" t="s">
+      <c r="D5" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="E5" s="59" t="s">
+      <c r="E5" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="F5" s="73" t="s">
+      <c r="F5" s="33" t="s">
         <v>119</v>
       </c>
-      <c r="G5" s="73" t="s">
+      <c r="G5" s="33" t="s">
         <v>120</v>
       </c>
-      <c r="H5" s="73" t="s">
+      <c r="H5" s="33" t="s">
         <v>121</v>
       </c>
-      <c r="I5" s="72"/>
+      <c r="I5" s="41"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
@@ -4002,31 +4097,31 @@
       <c r="V5" s="4"/>
     </row>
     <row r="6" spans="1:22" ht="63">
-      <c r="A6" s="56" t="s">
+      <c r="A6" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="B6" s="71" t="s">
+      <c r="B6" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="C6" s="59" t="s">
+      <c r="C6" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="D6" s="59" t="s">
+      <c r="D6" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="E6" s="59" t="s">
+      <c r="E6" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="F6" s="73" t="s">
+      <c r="F6" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="G6" s="73" t="s">
+      <c r="G6" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="H6" s="73" t="s">
+      <c r="H6" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="72"/>
+      <c r="I6" s="41"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
@@ -4042,31 +4137,31 @@
       <c r="V6" s="4"/>
     </row>
     <row r="7" spans="1:22" ht="78.75">
-      <c r="A7" s="56" t="s">
+      <c r="A7" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="71" t="s">
+      <c r="B7" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="C7" s="59" t="s">
+      <c r="C7" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="D7" s="59" t="s">
+      <c r="D7" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="E7" s="59" t="s">
+      <c r="E7" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="F7" s="73" t="s">
+      <c r="F7" s="33" t="s">
         <v>124</v>
       </c>
-      <c r="G7" s="73" t="s">
+      <c r="G7" s="33" t="s">
         <v>124</v>
       </c>
-      <c r="H7" s="73" t="s">
+      <c r="H7" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="72"/>
+      <c r="I7" s="41"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
@@ -4082,31 +4177,31 @@
       <c r="V7" s="4"/>
     </row>
     <row r="8" spans="1:22" ht="31.5">
-      <c r="A8" s="56" t="s">
+      <c r="A8" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="B8" s="73" t="s">
+      <c r="B8" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="C8" s="59" t="s">
+      <c r="C8" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="D8" s="59" t="s">
+      <c r="D8" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="E8" s="59" t="s">
+      <c r="E8" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="F8" s="73" t="s">
+      <c r="F8" s="33" t="s">
         <v>125</v>
       </c>
-      <c r="G8" s="73" t="s">
+      <c r="G8" s="33" t="s">
         <v>125</v>
       </c>
-      <c r="H8" s="73" t="s">
+      <c r="H8" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="74"/>
+      <c r="I8" s="42"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
@@ -5744,8 +5839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -5759,307 +5854,307 @@
     <col min="7" max="7" width="33.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:9" ht="31.5">
+      <c r="A1" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="D1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="38" t="s">
+      <c r="E1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="38" t="s">
+      <c r="F1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="38" t="s">
+      <c r="G1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="38" t="s">
+      <c r="H1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="39" t="s">
+      <c r="I1" s="21" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="76.5">
-      <c r="A2" s="37" t="s">
+    <row r="2" spans="1:9" ht="94.5">
+      <c r="A2" s="53" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="21" t="str">
+      <c r="H2" s="53" t="str">
         <f xml:space="preserve"> IF(F2=G2, "Pass","Fail")</f>
         <v>Pass</v>
       </c>
-      <c r="I2" s="35" t="s">
+      <c r="I2" s="55" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="76.5">
-      <c r="A3" s="37" t="s">
+    <row r="3" spans="1:9" ht="94.5">
+      <c r="A3" s="53" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="52" t="s">
         <v>44</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="52" t="s">
         <v>44</v>
       </c>
-      <c r="H3" s="21" t="str">
+      <c r="H3" s="53" t="str">
         <f xml:space="preserve"> IF(F3=G3, "Pass","Fail")</f>
         <v>Pass</v>
       </c>
-      <c r="I3" s="35"/>
-    </row>
-    <row r="4" spans="1:9" ht="76.5">
-      <c r="A4" s="37" t="s">
+      <c r="I3" s="55"/>
+    </row>
+    <row r="4" spans="1:9" ht="94.5">
+      <c r="A4" s="53" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="54" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="51" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="20" t="s">
+      <c r="G4" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="21" t="str">
+      <c r="H4" s="53" t="str">
         <f xml:space="preserve"> IF(F4=G4, "Pass","Fail")</f>
         <v>Pass</v>
       </c>
-      <c r="I4" s="35"/>
-    </row>
-    <row r="5" spans="1:9" ht="76.5">
-      <c r="A5" s="37" t="s">
+      <c r="I4" s="55"/>
+    </row>
+    <row r="5" spans="1:9" ht="94.5">
+      <c r="A5" s="53" t="s">
         <v>76</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="20" t="s">
+      <c r="F5" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="H5" s="21" t="str">
+      <c r="H5" s="53" t="str">
         <f t="shared" ref="H5" si="0" xml:space="preserve"> IF(F5=G5, "Pass","Fail")</f>
         <v>Pass</v>
       </c>
-      <c r="I5" s="35"/>
-    </row>
-    <row r="6" spans="1:9" ht="78.75">
-      <c r="A6" s="37" t="s">
+      <c r="I5" s="55"/>
+    </row>
+    <row r="6" spans="1:9" ht="94.5">
+      <c r="A6" s="53" t="s">
         <v>78</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="20" t="s">
+      <c r="F6" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="G6" s="20" t="s">
+      <c r="G6" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="H6" s="21" t="s">
+      <c r="H6" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="35"/>
-    </row>
-    <row r="7" spans="1:9" ht="78.75">
-      <c r="A7" s="37" t="s">
+      <c r="I6" s="55"/>
+    </row>
+    <row r="7" spans="1:9" ht="94.5">
+      <c r="A7" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="G7" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="H7" s="21" t="s">
+      <c r="H7" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="35"/>
-    </row>
-    <row r="8" spans="1:9" ht="76.5">
-      <c r="A8" s="37" t="s">
+      <c r="I7" s="55"/>
+    </row>
+    <row r="8" spans="1:9" ht="94.5">
+      <c r="A8" s="53" t="s">
         <v>99</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="54" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="20" t="s">
+      <c r="F8" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="G8" s="20" t="s">
+      <c r="G8" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="H8" s="21" t="s">
+      <c r="H8" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="35"/>
+      <c r="I8" s="55"/>
     </row>
     <row r="9" spans="1:9" ht="78.75">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="53" t="s">
         <v>101</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="20" t="s">
+      <c r="F9" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="20" t="s">
+      <c r="G9" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="21" t="str">
+      <c r="H9" s="53" t="str">
         <f t="shared" ref="H9" si="1" xml:space="preserve"> IF(F9=G9, "Pass","Fail")</f>
         <v>Pass</v>
       </c>
-      <c r="I9" s="35"/>
+      <c r="I9" s="55"/>
     </row>
     <row r="10" spans="1:9" ht="63">
-      <c r="A10" s="37" t="s">
+      <c r="A10" s="53" t="s">
         <v>102</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="19"/>
-      <c r="F10" s="20" t="s">
+      <c r="E10" s="51"/>
+      <c r="F10" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="G10" s="20" t="s">
+      <c r="G10" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="H10" s="21" t="s">
+      <c r="H10" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="I10" s="35"/>
+      <c r="I10" s="55"/>
     </row>
     <row r="11" spans="1:9" ht="63">
-      <c r="A11" s="37" t="s">
+      <c r="A11" s="53" t="s">
         <v>104</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="D11" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="19"/>
-      <c r="F11" s="20" t="s">
+      <c r="E11" s="51"/>
+      <c r="F11" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="G11" s="20" t="s">
+      <c r="G11" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="H11" s="21" t="s">
+      <c r="H11" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="I11" s="35"/>
+      <c r="I11" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -6074,8 +6169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A12"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D12" sqref="A1:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -6089,340 +6184,340 @@
     <col min="7" max="7" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="46" customFormat="1" ht="25.5">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:9" s="17" customFormat="1" ht="31.5">
+      <c r="A1" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="D1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="38" t="s">
+      <c r="E1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="38" t="s">
+      <c r="F1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="38" t="s">
+      <c r="G1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="38" t="s">
+      <c r="H1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="39" t="s">
+      <c r="I1" s="21" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="76.5">
-      <c r="A2" s="47" t="s">
+    <row r="2" spans="1:9" ht="157.5">
+      <c r="A2" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="65" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="42" t="s">
+      <c r="D2" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="43" t="s">
+      <c r="E2" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="44" t="s">
+      <c r="F2" s="59" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="44" t="s">
+      <c r="G2" s="59" t="s">
         <v>54</v>
       </c>
-      <c r="H2" s="45" t="str">
+      <c r="H2" s="60" t="str">
         <f xml:space="preserve"> IF(F2=G2, "Pass","Fail")</f>
         <v>Pass</v>
       </c>
-      <c r="I2" s="31" t="s">
+      <c r="I2" s="66" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="76.5">
-      <c r="A3" s="47" t="s">
+    <row r="3" spans="1:9" ht="157.5">
+      <c r="A3" s="64" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="15" t="s">
         <v>53</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="61" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="H3" s="9" t="str">
+      <c r="H3" s="63" t="str">
         <f xml:space="preserve"> IF(F3=G3, "Pass","Fail")</f>
         <v>Pass</v>
       </c>
-      <c r="I3" s="32"/>
-    </row>
-    <row r="4" spans="1:9" ht="76.5">
-      <c r="A4" s="47" t="s">
+      <c r="I3" s="67"/>
+    </row>
+    <row r="4" spans="1:9" ht="157.5">
+      <c r="A4" s="64" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="15" t="s">
         <v>53</v>
       </c>
       <c r="D4" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="61" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="9" t="str">
+      <c r="H4" s="63" t="str">
         <f xml:space="preserve"> IF(F4=G4, "Pass","Fail")</f>
         <v>Pass</v>
       </c>
-      <c r="I4" s="32"/>
-    </row>
-    <row r="5" spans="1:9" ht="76.5">
-      <c r="A5" s="47" t="s">
+      <c r="I4" s="67"/>
+    </row>
+    <row r="5" spans="1:9" ht="157.5">
+      <c r="A5" s="64" t="s">
         <v>76</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="15" t="s">
         <v>53</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="62" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="62" t="s">
         <v>64</v>
       </c>
-      <c r="H5" s="9" t="str">
+      <c r="H5" s="63" t="str">
         <f t="shared" ref="H5" si="0" xml:space="preserve"> IF(F5=G5, "Pass","Fail")</f>
         <v>Fail</v>
       </c>
-      <c r="I5" s="32"/>
-    </row>
-    <row r="6" spans="1:9" s="34" customFormat="1" ht="76.5">
-      <c r="A6" s="47" t="s">
+      <c r="I5" s="67"/>
+    </row>
+    <row r="6" spans="1:9" s="16" customFormat="1" ht="157.5">
+      <c r="A6" s="64" t="s">
         <v>78</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="54" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="F6" s="20" t="s">
+      <c r="F6" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="G6" s="20" t="s">
+      <c r="G6" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="H6" s="21" t="str">
+      <c r="H6" s="53" t="str">
         <f t="shared" ref="H6:H12" si="1" xml:space="preserve"> IF(F6=G6, "Pass","Fail")</f>
         <v>Fail</v>
       </c>
-      <c r="I6" s="32"/>
-    </row>
-    <row r="7" spans="1:9" ht="76.5">
-      <c r="A7" s="47" t="s">
+      <c r="I6" s="67"/>
+    </row>
+    <row r="7" spans="1:9" ht="141.75">
+      <c r="A7" s="64" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="15" t="s">
         <v>53</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="62" t="s">
         <v>69</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="62" t="s">
         <v>66</v>
       </c>
-      <c r="H7" s="21" t="str">
+      <c r="H7" s="53" t="str">
         <f t="shared" si="1"/>
         <v>Fail</v>
       </c>
-      <c r="I7" s="32"/>
-    </row>
-    <row r="8" spans="1:9" ht="76.5">
-      <c r="A8" s="47" t="s">
+      <c r="I7" s="67"/>
+    </row>
+    <row r="8" spans="1:9" ht="157.5">
+      <c r="A8" s="64" t="s">
         <v>99</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="15" t="s">
         <v>53</v>
       </c>
       <c r="D8" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="62" t="s">
         <v>70</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="G8" s="62" t="s">
         <v>67</v>
       </c>
-      <c r="H8" s="21" t="str">
+      <c r="H8" s="53" t="str">
         <f t="shared" si="1"/>
         <v>Fail</v>
       </c>
-      <c r="I8" s="32"/>
-    </row>
-    <row r="9" spans="1:9" ht="76.5">
-      <c r="A9" s="47" t="s">
+      <c r="I8" s="67"/>
+    </row>
+    <row r="9" spans="1:9" ht="157.5">
+      <c r="A9" s="64" t="s">
         <v>101</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="15" t="s">
         <v>53</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="H9" s="21" t="str">
+      <c r="H9" s="53" t="str">
         <f t="shared" si="1"/>
         <v>Pass</v>
       </c>
-      <c r="I9" s="32"/>
+      <c r="I9" s="67"/>
     </row>
     <row r="10" spans="1:9" ht="78.75">
-      <c r="A10" s="47" t="s">
+      <c r="A10" s="64" t="s">
         <v>102</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="15" t="s">
         <v>53</v>
       </c>
       <c r="D10" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="61" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="12" t="s">
+      <c r="G10" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="H10" s="21" t="str">
+      <c r="H10" s="53" t="str">
         <f t="shared" si="1"/>
         <v>Pass</v>
       </c>
-      <c r="I10" s="32"/>
+      <c r="I10" s="67"/>
     </row>
     <row r="11" spans="1:9" ht="63">
-      <c r="A11" s="47" t="s">
+      <c r="A11" s="64" t="s">
         <v>104</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="15" t="s">
         <v>53</v>
       </c>
       <c r="D11" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="12" t="s">
+      <c r="E11" s="61"/>
+      <c r="F11" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="G11" s="12" t="s">
+      <c r="G11" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="H11" s="21" t="str">
+      <c r="H11" s="53" t="str">
         <f t="shared" si="1"/>
         <v>Pass</v>
       </c>
-      <c r="I11" s="32"/>
+      <c r="I11" s="67"/>
     </row>
     <row r="12" spans="1:9" ht="63">
-      <c r="A12" s="47" t="s">
+      <c r="A12" s="64" t="s">
         <v>106</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="68" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="15" t="s">
         <v>53</v>
       </c>
       <c r="D12" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="11"/>
-      <c r="F12" s="12" t="s">
+      <c r="E12" s="61"/>
+      <c r="F12" s="62" t="s">
         <v>38</v>
       </c>
-      <c r="G12" s="12" t="s">
+      <c r="G12" s="62" t="s">
         <v>38</v>
       </c>
-      <c r="H12" s="21" t="str">
+      <c r="H12" s="53" t="str">
         <f t="shared" si="1"/>
         <v>Pass</v>
       </c>
-      <c r="I12" s="33"/>
+      <c r="I12" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -6437,8 +6532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V95"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D10" sqref="A1:I29"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75"/>
@@ -6454,31 +6549,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="8" customFormat="1" ht="15.75">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="60" t="s">
+      <c r="C1" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="60" t="s">
+      <c r="D1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="60" t="s">
+      <c r="E1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="60" t="s">
+      <c r="F1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="60" t="s">
+      <c r="G1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="60" t="s">
+      <c r="H1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="61" t="s">
+      <c r="I1" s="26" t="s">
         <v>13</v>
       </c>
       <c r="J1" s="7"/>
@@ -6496,23 +6591,27 @@
       <c r="V1" s="7"/>
     </row>
     <row r="2" spans="1:22" ht="47.25">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="64" t="s">
+      <c r="B2" s="35" t="s">
+        <v>294</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D2" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64" t="s">
+      <c r="E2" s="29"/>
+      <c r="F2" s="29" t="s">
         <v>134</v>
       </c>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63" t="s">
+      <c r="G2" s="28"/>
+      <c r="H2" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="65" t="s">
+      <c r="I2" s="43" t="s">
         <v>135</v>
       </c>
       <c r="J2" s="3"/>
@@ -6529,26 +6628,30 @@
       <c r="U2" s="3"/>
       <c r="V2" s="3"/>
     </row>
-    <row r="3" spans="1:22" ht="31.5">
-      <c r="A3" s="62" t="s">
+    <row r="3" spans="1:22" ht="47.25">
+      <c r="A3" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="63"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="66" t="s">
+      <c r="B3" s="35" t="s">
+        <v>295</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D3" s="30" t="s">
         <v>136</v>
       </c>
-      <c r="E3" s="66" t="s">
+      <c r="E3" s="30" t="s">
         <v>137</v>
       </c>
-      <c r="F3" s="66" t="s">
+      <c r="F3" s="30" t="s">
         <v>138</v>
       </c>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63" t="s">
+      <c r="G3" s="28"/>
+      <c r="H3" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="67"/>
+      <c r="I3" s="44"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -6564,25 +6667,29 @@
       <c r="V3" s="3"/>
     </row>
     <row r="4" spans="1:22" ht="47.25">
-      <c r="A4" s="62" t="s">
+      <c r="A4" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="63"/>
-      <c r="C4" s="63"/>
-      <c r="D4" s="66" t="s">
+      <c r="B4" s="35" t="s">
+        <v>296</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D4" s="30" t="s">
         <v>139</v>
       </c>
-      <c r="E4" s="66" t="s">
+      <c r="E4" s="30" t="s">
         <v>140</v>
       </c>
-      <c r="F4" s="66" t="s">
+      <c r="F4" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="G4" s="63"/>
-      <c r="H4" s="63" t="s">
+      <c r="G4" s="28"/>
+      <c r="H4" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="67"/>
+      <c r="I4" s="44"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
@@ -6598,23 +6705,27 @@
       <c r="V4" s="3"/>
     </row>
     <row r="5" spans="1:22" ht="47.25">
-      <c r="A5" s="62" t="s">
+      <c r="A5" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="B5" s="63"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="66" t="s">
+      <c r="B5" s="35" t="s">
+        <v>297</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D5" s="30" t="s">
         <v>142</v>
       </c>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66" t="s">
+      <c r="E5" s="30"/>
+      <c r="F5" s="30" t="s">
         <v>143</v>
       </c>
-      <c r="G5" s="63"/>
-      <c r="H5" s="63" t="s">
+      <c r="G5" s="28"/>
+      <c r="H5" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="67"/>
+      <c r="I5" s="44"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
@@ -6630,23 +6741,27 @@
       <c r="V5" s="3"/>
     </row>
     <row r="6" spans="1:22" ht="47.25">
-      <c r="A6" s="62" t="s">
+      <c r="A6" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="B6" s="63"/>
-      <c r="C6" s="63"/>
-      <c r="D6" s="64" t="s">
+      <c r="B6" s="35" t="s">
+        <v>298</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D6" s="29" t="s">
         <v>144</v>
       </c>
-      <c r="E6" s="64"/>
-      <c r="F6" s="64" t="s">
+      <c r="E6" s="29"/>
+      <c r="F6" s="29" t="s">
         <v>145</v>
       </c>
-      <c r="G6" s="63"/>
-      <c r="H6" s="63" t="s">
+      <c r="G6" s="28"/>
+      <c r="H6" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="67"/>
+      <c r="I6" s="44"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
@@ -6662,23 +6777,27 @@
       <c r="V6" s="3"/>
     </row>
     <row r="7" spans="1:22" ht="47.25">
-      <c r="A7" s="62" t="s">
+      <c r="A7" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="63"/>
-      <c r="C7" s="63"/>
-      <c r="D7" s="66" t="s">
+      <c r="B7" s="35" t="s">
+        <v>299</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D7" s="30" t="s">
         <v>142</v>
       </c>
-      <c r="E7" s="66"/>
-      <c r="F7" s="66" t="s">
+      <c r="E7" s="30"/>
+      <c r="F7" s="30" t="s">
         <v>143</v>
       </c>
-      <c r="G7" s="63"/>
-      <c r="H7" s="63" t="s">
+      <c r="G7" s="28"/>
+      <c r="H7" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="67"/>
+      <c r="I7" s="44"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
@@ -6694,23 +6813,27 @@
       <c r="V7" s="3"/>
     </row>
     <row r="8" spans="1:22" ht="47.25">
-      <c r="A8" s="62" t="s">
+      <c r="A8" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="B8" s="63"/>
-      <c r="C8" s="63"/>
-      <c r="D8" s="64" t="s">
+      <c r="B8" s="35" t="s">
+        <v>300</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D8" s="29" t="s">
         <v>146</v>
       </c>
-      <c r="E8" s="64"/>
-      <c r="F8" s="64" t="s">
+      <c r="E8" s="29"/>
+      <c r="F8" s="29" t="s">
         <v>147</v>
       </c>
-      <c r="G8" s="63"/>
-      <c r="H8" s="63" t="s">
+      <c r="G8" s="28"/>
+      <c r="H8" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="67"/>
+      <c r="I8" s="44"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
@@ -6725,26 +6848,30 @@
       <c r="U8" s="3"/>
       <c r="V8" s="3"/>
     </row>
-    <row r="9" spans="1:22" ht="31.5">
-      <c r="A9" s="62" t="s">
+    <row r="9" spans="1:22" ht="47.25">
+      <c r="A9" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="B9" s="63"/>
-      <c r="C9" s="63"/>
-      <c r="D9" s="66" t="s">
+      <c r="B9" s="35" t="s">
+        <v>301</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D9" s="30" t="s">
         <v>148</v>
       </c>
-      <c r="E9" s="66" t="s">
+      <c r="E9" s="30" t="s">
         <v>149</v>
       </c>
-      <c r="F9" s="66" t="s">
+      <c r="F9" s="30" t="s">
         <v>138</v>
       </c>
-      <c r="G9" s="63"/>
-      <c r="H9" s="63" t="s">
+      <c r="G9" s="28"/>
+      <c r="H9" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="I9" s="67"/>
+      <c r="I9" s="44"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
@@ -6760,25 +6887,29 @@
       <c r="V9" s="3"/>
     </row>
     <row r="10" spans="1:22" ht="47.25">
-      <c r="A10" s="62" t="s">
+      <c r="A10" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="B10" s="63"/>
-      <c r="C10" s="63"/>
-      <c r="D10" s="66" t="s">
+      <c r="B10" s="35" t="s">
+        <v>302</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D10" s="30" t="s">
         <v>150</v>
       </c>
-      <c r="E10" s="66" t="s">
+      <c r="E10" s="30" t="s">
         <v>151</v>
       </c>
-      <c r="F10" s="66" t="s">
+      <c r="F10" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="G10" s="63"/>
-      <c r="H10" s="63" t="s">
+      <c r="G10" s="28"/>
+      <c r="H10" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="I10" s="67"/>
+      <c r="I10" s="44"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
@@ -6794,23 +6925,27 @@
       <c r="V10" s="3"/>
     </row>
     <row r="11" spans="1:22" ht="47.25">
-      <c r="A11" s="62" t="s">
+      <c r="A11" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="B11" s="63"/>
-      <c r="C11" s="63"/>
-      <c r="D11" s="66" t="s">
+      <c r="B11" s="35" t="s">
+        <v>303</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D11" s="30" t="s">
         <v>142</v>
       </c>
-      <c r="E11" s="66"/>
-      <c r="F11" s="66" t="s">
+      <c r="E11" s="30"/>
+      <c r="F11" s="30" t="s">
         <v>143</v>
       </c>
-      <c r="G11" s="63"/>
-      <c r="H11" s="63" t="s">
+      <c r="G11" s="28"/>
+      <c r="H11" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="I11" s="67"/>
+      <c r="I11" s="44"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
@@ -6825,24 +6960,28 @@
       <c r="U11" s="3"/>
       <c r="V11" s="3"/>
     </row>
-    <row r="12" spans="1:22" ht="31.5">
-      <c r="A12" s="62" t="s">
+    <row r="12" spans="1:22" ht="47.25">
+      <c r="A12" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="B12" s="63"/>
-      <c r="C12" s="63"/>
-      <c r="D12" s="64" t="s">
+      <c r="B12" s="36" t="s">
+        <v>304</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D12" s="29" t="s">
         <v>152</v>
       </c>
-      <c r="E12" s="64"/>
-      <c r="F12" s="64" t="s">
+      <c r="E12" s="29"/>
+      <c r="F12" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="G12" s="63"/>
-      <c r="H12" s="63" t="s">
+      <c r="G12" s="28"/>
+      <c r="H12" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="I12" s="67"/>
+      <c r="I12" s="44"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
@@ -6857,26 +6996,30 @@
       <c r="U12" s="3"/>
       <c r="V12" s="3"/>
     </row>
-    <row r="13" spans="1:22" ht="31.5">
-      <c r="A13" s="62" t="s">
+    <row r="13" spans="1:22" ht="47.25">
+      <c r="A13" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="B13" s="63"/>
-      <c r="C13" s="63"/>
-      <c r="D13" s="66" t="s">
+      <c r="B13" s="36" t="s">
+        <v>305</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D13" s="30" t="s">
         <v>154</v>
       </c>
-      <c r="E13" s="66" t="s">
+      <c r="E13" s="30" t="s">
         <v>155</v>
       </c>
-      <c r="F13" s="66" t="s">
+      <c r="F13" s="30" t="s">
         <v>138</v>
       </c>
-      <c r="G13" s="63"/>
-      <c r="H13" s="63" t="s">
+      <c r="G13" s="28"/>
+      <c r="H13" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="I13" s="67"/>
+      <c r="I13" s="44"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
@@ -6892,25 +7035,29 @@
       <c r="V13" s="3"/>
     </row>
     <row r="14" spans="1:22" ht="47.25">
-      <c r="A14" s="62" t="s">
+      <c r="A14" s="27" t="s">
         <v>242</v>
       </c>
-      <c r="B14" s="63"/>
-      <c r="C14" s="63"/>
-      <c r="D14" s="66" t="s">
+      <c r="B14" s="36" t="s">
+        <v>306</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D14" s="30" t="s">
         <v>156</v>
       </c>
-      <c r="E14" s="66" t="s">
+      <c r="E14" s="30" t="s">
         <v>157</v>
       </c>
-      <c r="F14" s="66" t="s">
+      <c r="F14" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="G14" s="63"/>
-      <c r="H14" s="63" t="s">
+      <c r="G14" s="28"/>
+      <c r="H14" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="I14" s="67"/>
+      <c r="I14" s="44"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
@@ -6926,23 +7073,27 @@
       <c r="V14" s="3"/>
     </row>
     <row r="15" spans="1:22" ht="47.25">
-      <c r="A15" s="62" t="s">
+      <c r="A15" s="27" t="s">
         <v>244</v>
       </c>
-      <c r="B15" s="63"/>
-      <c r="C15" s="63"/>
-      <c r="D15" s="66" t="s">
+      <c r="B15" s="36" t="s">
+        <v>307</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D15" s="30" t="s">
         <v>142</v>
       </c>
-      <c r="E15" s="66"/>
-      <c r="F15" s="66" t="s">
+      <c r="E15" s="30"/>
+      <c r="F15" s="30" t="s">
         <v>143</v>
       </c>
-      <c r="G15" s="63"/>
-      <c r="H15" s="63" t="s">
+      <c r="G15" s="28"/>
+      <c r="H15" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="I15" s="67"/>
+      <c r="I15" s="44"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
@@ -6957,26 +7108,30 @@
       <c r="U15" s="3"/>
       <c r="V15" s="3"/>
     </row>
-    <row r="16" spans="1:22" ht="31.5">
-      <c r="A16" s="62" t="s">
+    <row r="16" spans="1:22" ht="47.25">
+      <c r="A16" s="27" t="s">
         <v>279</v>
       </c>
-      <c r="B16" s="63"/>
-      <c r="C16" s="63"/>
-      <c r="D16" s="64" t="s">
+      <c r="B16" s="36" t="s">
+        <v>308</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D16" s="29" t="s">
         <v>158</v>
       </c>
-      <c r="E16" s="64" t="s">
+      <c r="E16" s="29" t="s">
         <v>159</v>
       </c>
-      <c r="F16" s="64" t="s">
+      <c r="F16" s="29" t="s">
         <v>160</v>
       </c>
-      <c r="G16" s="63"/>
-      <c r="H16" s="63" t="s">
+      <c r="G16" s="28"/>
+      <c r="H16" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="I16" s="67"/>
+      <c r="I16" s="44"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
@@ -6992,23 +7147,27 @@
       <c r="V16" s="3"/>
     </row>
     <row r="17" spans="1:22" ht="47.25">
-      <c r="A17" s="62" t="s">
+      <c r="A17" s="27" t="s">
         <v>280</v>
       </c>
-      <c r="B17" s="63"/>
-      <c r="C17" s="63"/>
-      <c r="D17" s="66" t="s">
+      <c r="B17" s="36" t="s">
+        <v>309</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D17" s="30" t="s">
         <v>161</v>
       </c>
-      <c r="E17" s="66"/>
-      <c r="F17" s="66" t="s">
+      <c r="E17" s="30"/>
+      <c r="F17" s="30" t="s">
         <v>162</v>
       </c>
-      <c r="G17" s="63"/>
-      <c r="H17" s="63" t="s">
+      <c r="G17" s="28"/>
+      <c r="H17" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="I17" s="67"/>
+      <c r="I17" s="44"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
@@ -7024,25 +7183,29 @@
       <c r="V17" s="3"/>
     </row>
     <row r="18" spans="1:22" ht="47.25">
-      <c r="A18" s="62" t="s">
+      <c r="A18" s="27" t="s">
         <v>281</v>
       </c>
-      <c r="B18" s="63"/>
-      <c r="C18" s="63"/>
-      <c r="D18" s="66" t="s">
+      <c r="B18" s="36" t="s">
+        <v>310</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D18" s="30" t="s">
         <v>163</v>
       </c>
-      <c r="E18" s="66" t="s">
+      <c r="E18" s="30" t="s">
         <v>164</v>
       </c>
-      <c r="F18" s="66" t="s">
+      <c r="F18" s="30" t="s">
         <v>165</v>
       </c>
-      <c r="G18" s="63"/>
-      <c r="H18" s="63" t="s">
+      <c r="G18" s="28"/>
+      <c r="H18" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="I18" s="67"/>
+      <c r="I18" s="44"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
@@ -7058,25 +7221,29 @@
       <c r="V18" s="3"/>
     </row>
     <row r="19" spans="1:22" ht="47.25">
-      <c r="A19" s="62" t="s">
+      <c r="A19" s="27" t="s">
         <v>282</v>
       </c>
-      <c r="B19" s="63"/>
-      <c r="C19" s="63"/>
-      <c r="D19" s="66" t="s">
+      <c r="B19" s="36" t="s">
+        <v>311</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D19" s="30" t="s">
         <v>166</v>
       </c>
-      <c r="E19" s="66" t="s">
+      <c r="E19" s="30" t="s">
         <v>167</v>
       </c>
-      <c r="F19" s="66" t="s">
+      <c r="F19" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="G19" s="63"/>
-      <c r="H19" s="63" t="s">
+      <c r="G19" s="28"/>
+      <c r="H19" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="I19" s="67"/>
+      <c r="I19" s="44"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
@@ -7092,23 +7259,27 @@
       <c r="V19" s="3"/>
     </row>
     <row r="20" spans="1:22" ht="47.25">
-      <c r="A20" s="62" t="s">
+      <c r="A20" s="27" t="s">
         <v>283</v>
       </c>
-      <c r="B20" s="63"/>
-      <c r="C20" s="63"/>
-      <c r="D20" s="66" t="s">
+      <c r="B20" s="36" t="s">
+        <v>312</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D20" s="30" t="s">
         <v>142</v>
       </c>
-      <c r="E20" s="66"/>
-      <c r="F20" s="66" t="s">
+      <c r="E20" s="30"/>
+      <c r="F20" s="30" t="s">
         <v>143</v>
       </c>
-      <c r="G20" s="63"/>
-      <c r="H20" s="63" t="s">
+      <c r="G20" s="28"/>
+      <c r="H20" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="I20" s="67"/>
+      <c r="I20" s="44"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
@@ -7123,24 +7294,28 @@
       <c r="U20" s="3"/>
       <c r="V20" s="3"/>
     </row>
-    <row r="21" spans="1:22" ht="31.5">
-      <c r="A21" s="62" t="s">
+    <row r="21" spans="1:22" ht="47.25">
+      <c r="A21" s="27" t="s">
         <v>284</v>
       </c>
-      <c r="B21" s="63"/>
-      <c r="C21" s="63"/>
-      <c r="D21" s="66" t="s">
+      <c r="B21" s="36" t="s">
+        <v>313</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D21" s="30" t="s">
         <v>142</v>
       </c>
-      <c r="E21" s="66"/>
-      <c r="F21" s="66" t="s">
+      <c r="E21" s="30"/>
+      <c r="F21" s="30" t="s">
         <v>168</v>
       </c>
-      <c r="G21" s="63"/>
-      <c r="H21" s="63" t="s">
+      <c r="G21" s="28"/>
+      <c r="H21" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="I21" s="67"/>
+      <c r="I21" s="44"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
@@ -7156,23 +7331,27 @@
       <c r="V21" s="3"/>
     </row>
     <row r="22" spans="1:22" ht="47.25">
-      <c r="A22" s="62" t="s">
+      <c r="A22" s="27" t="s">
         <v>285</v>
       </c>
-      <c r="B22" s="63"/>
-      <c r="C22" s="63"/>
-      <c r="D22" s="64" t="s">
+      <c r="B22" s="36" t="s">
+        <v>314</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D22" s="29" t="s">
         <v>169</v>
       </c>
-      <c r="E22" s="64"/>
-      <c r="F22" s="64" t="s">
+      <c r="E22" s="29"/>
+      <c r="F22" s="29" t="s">
         <v>170</v>
       </c>
-      <c r="G22" s="63"/>
-      <c r="H22" s="63" t="s">
+      <c r="G22" s="28"/>
+      <c r="H22" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="I22" s="67"/>
+      <c r="I22" s="44"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
@@ -7188,23 +7367,27 @@
       <c r="V22" s="3"/>
     </row>
     <row r="23" spans="1:22" ht="47.25">
-      <c r="A23" s="62" t="s">
+      <c r="A23" s="27" t="s">
         <v>286</v>
       </c>
-      <c r="B23" s="63"/>
-      <c r="C23" s="63"/>
-      <c r="D23" s="66" t="s">
+      <c r="B23" s="36" t="s">
+        <v>315</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D23" s="30" t="s">
         <v>142</v>
       </c>
-      <c r="E23" s="66"/>
-      <c r="F23" s="66" t="s">
+      <c r="E23" s="30"/>
+      <c r="F23" s="30" t="s">
         <v>143</v>
       </c>
-      <c r="G23" s="63"/>
-      <c r="H23" s="63" t="s">
+      <c r="G23" s="28"/>
+      <c r="H23" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="I23" s="67"/>
+      <c r="I23" s="44"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
@@ -7220,25 +7403,29 @@
       <c r="V23" s="3"/>
     </row>
     <row r="24" spans="1:22" ht="47.25">
-      <c r="A24" s="62" t="s">
+      <c r="A24" s="27" t="s">
         <v>287</v>
       </c>
-      <c r="B24" s="63"/>
-      <c r="C24" s="63"/>
-      <c r="D24" s="66" t="s">
+      <c r="B24" s="36" t="s">
+        <v>316</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D24" s="30" t="s">
         <v>171</v>
       </c>
-      <c r="E24" s="66" t="s">
+      <c r="E24" s="30" t="s">
         <v>172</v>
       </c>
-      <c r="F24" s="66" t="s">
+      <c r="F24" s="30" t="s">
         <v>173</v>
       </c>
-      <c r="G24" s="63"/>
-      <c r="H24" s="63" t="s">
+      <c r="G24" s="28"/>
+      <c r="H24" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="I24" s="67"/>
+      <c r="I24" s="44"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
@@ -7254,25 +7441,29 @@
       <c r="V24" s="3"/>
     </row>
     <row r="25" spans="1:22" ht="47.25">
-      <c r="A25" s="62" t="s">
+      <c r="A25" s="27" t="s">
         <v>288</v>
       </c>
-      <c r="B25" s="63"/>
-      <c r="C25" s="63"/>
-      <c r="D25" s="66" t="s">
+      <c r="B25" s="36" t="s">
+        <v>317</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D25" s="30" t="s">
         <v>174</v>
       </c>
-      <c r="E25" s="66" t="s">
+      <c r="E25" s="30" t="s">
         <v>175</v>
       </c>
-      <c r="F25" s="66" t="s">
+      <c r="F25" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="G25" s="63"/>
-      <c r="H25" s="63" t="s">
+      <c r="G25" s="28"/>
+      <c r="H25" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="I25" s="67"/>
+      <c r="I25" s="44"/>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
@@ -7288,23 +7479,27 @@
       <c r="V25" s="3"/>
     </row>
     <row r="26" spans="1:22" ht="47.25">
-      <c r="A26" s="62" t="s">
+      <c r="A26" s="27" t="s">
         <v>289</v>
       </c>
-      <c r="B26" s="63"/>
-      <c r="C26" s="63"/>
-      <c r="D26" s="64" t="s">
+      <c r="B26" s="36" t="s">
+        <v>318</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D26" s="29" t="s">
         <v>176</v>
       </c>
-      <c r="E26" s="64"/>
-      <c r="F26" s="64" t="s">
+      <c r="E26" s="29"/>
+      <c r="F26" s="29" t="s">
         <v>177</v>
       </c>
-      <c r="G26" s="63"/>
-      <c r="H26" s="63" t="s">
+      <c r="G26" s="28"/>
+      <c r="H26" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="I26" s="67"/>
+      <c r="I26" s="44"/>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
@@ -7320,25 +7515,29 @@
       <c r="V26" s="3"/>
     </row>
     <row r="27" spans="1:22" ht="78.75">
-      <c r="A27" s="62" t="s">
+      <c r="A27" s="27" t="s">
         <v>290</v>
       </c>
-      <c r="B27" s="63"/>
-      <c r="C27" s="63"/>
-      <c r="D27" s="66" t="s">
+      <c r="B27" s="36" t="s">
+        <v>319</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D27" s="30" t="s">
         <v>178</v>
       </c>
-      <c r="E27" s="66" t="s">
+      <c r="E27" s="30" t="s">
         <v>179</v>
       </c>
-      <c r="F27" s="66" t="s">
+      <c r="F27" s="30" t="s">
         <v>180</v>
       </c>
-      <c r="G27" s="63"/>
-      <c r="H27" s="63" t="s">
+      <c r="G27" s="28"/>
+      <c r="H27" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="I27" s="67"/>
+      <c r="I27" s="44"/>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
@@ -7353,24 +7552,28 @@
       <c r="U27" s="3"/>
       <c r="V27" s="3"/>
     </row>
-    <row r="28" spans="1:22" ht="31.5">
-      <c r="A28" s="62" t="s">
+    <row r="28" spans="1:22" ht="47.25">
+      <c r="A28" s="27" t="s">
         <v>291</v>
       </c>
-      <c r="B28" s="63"/>
-      <c r="C28" s="63"/>
-      <c r="D28" s="66" t="s">
+      <c r="B28" s="36" t="s">
+        <v>320</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D28" s="30" t="s">
         <v>181</v>
       </c>
-      <c r="E28" s="66"/>
-      <c r="F28" s="66" t="s">
+      <c r="E28" s="30"/>
+      <c r="F28" s="30" t="s">
         <v>182</v>
       </c>
-      <c r="G28" s="63"/>
-      <c r="H28" s="63" t="s">
+      <c r="G28" s="28"/>
+      <c r="H28" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="I28" s="67"/>
+      <c r="I28" s="44"/>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
@@ -7386,23 +7589,27 @@
       <c r="V28" s="3"/>
     </row>
     <row r="29" spans="1:22" ht="173.25">
-      <c r="A29" s="62" t="s">
+      <c r="A29" s="27" t="s">
         <v>292</v>
       </c>
-      <c r="B29" s="63"/>
-      <c r="C29" s="63"/>
-      <c r="D29" s="66" t="s">
+      <c r="B29" s="36" t="s">
+        <v>321</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D29" s="30" t="s">
         <v>183</v>
       </c>
-      <c r="E29" s="66"/>
-      <c r="F29" s="68" t="s">
+      <c r="E29" s="30"/>
+      <c r="F29" s="31" t="s">
         <v>184</v>
       </c>
-      <c r="G29" s="63"/>
-      <c r="H29" s="63" t="s">
+      <c r="G29" s="28"/>
+      <c r="H29" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="I29" s="69"/>
+      <c r="I29" s="45"/>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
@@ -8393,7 +8600,7 @@
   <dimension ref="A1:V95"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75"/>
@@ -8450,24 +8657,28 @@
       <c r="U1" s="7"/>
       <c r="V1" s="7"/>
     </row>
-    <row r="2" spans="1:22" ht="31.5">
-      <c r="A2" s="22" t="s">
+    <row r="2" spans="1:22" ht="47.25">
+      <c r="A2" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="49" t="s">
+      <c r="B2" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>331</v>
+      </c>
+      <c r="D2" s="18" t="s">
         <v>185</v>
       </c>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49" t="s">
+      <c r="E2" s="18"/>
+      <c r="F2" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50" t="s">
+      <c r="G2" s="19"/>
+      <c r="H2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="51" t="s">
+      <c r="I2" s="46" t="s">
         <v>135</v>
       </c>
       <c r="J2" s="3"/>
@@ -8485,25 +8696,29 @@
       <c r="V2" s="3"/>
     </row>
     <row r="3" spans="1:22" ht="47.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="49" t="s">
+      <c r="B3" s="36" t="s">
+        <v>323</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>331</v>
+      </c>
+      <c r="D3" s="18" t="s">
         <v>187</v>
       </c>
-      <c r="E3" s="49" t="s">
+      <c r="E3" s="18" t="s">
         <v>188</v>
       </c>
-      <c r="F3" s="49" t="s">
+      <c r="F3" s="18" t="s">
         <v>189</v>
       </c>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50" t="s">
+      <c r="G3" s="19"/>
+      <c r="H3" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="52"/>
+      <c r="I3" s="47"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -8519,25 +8734,29 @@
       <c r="V3" s="3"/>
     </row>
     <row r="4" spans="1:22" ht="47.25">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="48"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="49" t="s">
+      <c r="B4" s="36" t="s">
+        <v>324</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>331</v>
+      </c>
+      <c r="D4" s="18" t="s">
         <v>190</v>
       </c>
-      <c r="E4" s="49" t="s">
+      <c r="E4" s="18" t="s">
         <v>191</v>
       </c>
-      <c r="F4" s="49" t="s">
+      <c r="F4" s="18" t="s">
         <v>192</v>
       </c>
-      <c r="G4" s="50"/>
-      <c r="H4" s="50" t="s">
+      <c r="G4" s="19"/>
+      <c r="H4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="52"/>
+      <c r="I4" s="47"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
@@ -8553,25 +8772,29 @@
       <c r="V4" s="3"/>
     </row>
     <row r="5" spans="1:22" ht="47.25">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B5" s="48"/>
-      <c r="C5" s="48"/>
-      <c r="D5" s="49" t="s">
+      <c r="B5" s="36" t="s">
+        <v>325</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>331</v>
+      </c>
+      <c r="D5" s="18" t="s">
         <v>193</v>
       </c>
-      <c r="E5" s="49" t="s">
+      <c r="E5" s="18" t="s">
         <v>194</v>
       </c>
-      <c r="F5" s="49" t="s">
+      <c r="F5" s="18" t="s">
         <v>195</v>
       </c>
-      <c r="G5" s="50"/>
-      <c r="H5" s="50" t="s">
+      <c r="G5" s="19"/>
+      <c r="H5" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="52"/>
+      <c r="I5" s="47"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
@@ -8587,23 +8810,27 @@
       <c r="V5" s="3"/>
     </row>
     <row r="6" spans="1:22" ht="47.25">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="B6" s="48"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="49" t="s">
+      <c r="B6" s="36" t="s">
+        <v>326</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>331</v>
+      </c>
+      <c r="D6" s="18" t="s">
         <v>196</v>
       </c>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49" t="s">
+      <c r="E6" s="18"/>
+      <c r="F6" s="18" t="s">
         <v>197</v>
       </c>
-      <c r="G6" s="50"/>
-      <c r="H6" s="50" t="s">
+      <c r="G6" s="19"/>
+      <c r="H6" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="52"/>
+      <c r="I6" s="47"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
@@ -8619,23 +8846,27 @@
       <c r="V6" s="3"/>
     </row>
     <row r="7" spans="1:22" ht="47.25">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="48"/>
-      <c r="C7" s="48"/>
-      <c r="D7" s="49" t="s">
+      <c r="B7" s="36" t="s">
+        <v>327</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>331</v>
+      </c>
+      <c r="D7" s="18" t="s">
         <v>198</v>
       </c>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49" t="s">
+      <c r="E7" s="18"/>
+      <c r="F7" s="18" t="s">
         <v>199</v>
       </c>
-      <c r="G7" s="50"/>
-      <c r="H7" s="50" t="s">
+      <c r="G7" s="19"/>
+      <c r="H7" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="52"/>
+      <c r="I7" s="47"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
@@ -8651,25 +8882,29 @@
       <c r="V7" s="3"/>
     </row>
     <row r="8" spans="1:22" ht="47.25">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="B8" s="48"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="49" t="s">
+      <c r="B8" s="36" t="s">
+        <v>328</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>331</v>
+      </c>
+      <c r="D8" s="18" t="s">
         <v>200</v>
       </c>
-      <c r="E8" s="49" t="s">
+      <c r="E8" s="18" t="s">
         <v>188</v>
       </c>
-      <c r="F8" s="49" t="s">
+      <c r="F8" s="18" t="s">
         <v>201</v>
       </c>
-      <c r="G8" s="50"/>
-      <c r="H8" s="50" t="s">
+      <c r="G8" s="19"/>
+      <c r="H8" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="52"/>
+      <c r="I8" s="47"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
@@ -8685,25 +8920,29 @@
       <c r="V8" s="3"/>
     </row>
     <row r="9" spans="1:22" ht="47.25">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="B9" s="48"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="49" t="s">
+      <c r="B9" s="36" t="s">
+        <v>329</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>331</v>
+      </c>
+      <c r="D9" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="E9" s="49" t="s">
+      <c r="E9" s="18" t="s">
         <v>191</v>
       </c>
-      <c r="F9" s="49" t="s">
+      <c r="F9" s="18" t="s">
         <v>203</v>
       </c>
-      <c r="G9" s="50"/>
-      <c r="H9" s="50" t="s">
+      <c r="G9" s="19"/>
+      <c r="H9" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="I9" s="52"/>
+      <c r="I9" s="47"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
@@ -8719,25 +8958,29 @@
       <c r="V9" s="3"/>
     </row>
     <row r="10" spans="1:22" ht="47.25">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="B10" s="48"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="49" t="s">
+      <c r="B10" s="36" t="s">
+        <v>330</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>331</v>
+      </c>
+      <c r="D10" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="E10" s="49" t="s">
+      <c r="E10" s="18" t="s">
         <v>194</v>
       </c>
-      <c r="F10" s="49" t="s">
+      <c r="F10" s="18" t="s">
         <v>205</v>
       </c>
-      <c r="G10" s="50"/>
-      <c r="H10" s="50" t="s">
+      <c r="G10" s="19"/>
+      <c r="H10" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="I10" s="52"/>
+      <c r="I10" s="47"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
@@ -8753,23 +8996,27 @@
       <c r="V10" s="3"/>
     </row>
     <row r="11" spans="1:22" ht="47.25">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="B11" s="48"/>
-      <c r="C11" s="48"/>
-      <c r="D11" s="49" t="s">
+      <c r="B11" s="36" t="s">
+        <v>326</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>331</v>
+      </c>
+      <c r="D11" s="18" t="s">
         <v>196</v>
       </c>
-      <c r="E11" s="49"/>
-      <c r="F11" s="49" t="s">
+      <c r="E11" s="18"/>
+      <c r="F11" s="18" t="s">
         <v>206</v>
       </c>
-      <c r="G11" s="50"/>
-      <c r="H11" s="50" t="s">
+      <c r="G11" s="19"/>
+      <c r="H11" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="I11" s="53"/>
+      <c r="I11" s="48"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
@@ -10191,8 +10438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V95"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A1:I14"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75"/>
@@ -10200,7 +10447,7 @@
     <col min="1" max="1" width="13" style="1" customWidth="1"/>
     <col min="2" max="3" width="38" style="1" customWidth="1"/>
     <col min="4" max="4" width="44.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23" style="1" customWidth="1"/>
+    <col min="5" max="5" width="36.140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="32.140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="23.5703125" style="1" customWidth="1"/>
     <col min="8" max="22" width="17.28515625" style="1" customWidth="1"/>
@@ -10208,31 +10455,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="8" customFormat="1" ht="15.75">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="54" t="s">
+      <c r="C1" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="54" t="s">
+      <c r="D1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="54" t="s">
+      <c r="E1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="54" t="s">
+      <c r="F1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="54" t="s">
+      <c r="G1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="54" t="s">
+      <c r="H1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="55" t="s">
+      <c r="I1" s="21" t="s">
         <v>13</v>
       </c>
       <c r="J1" s="7"/>
@@ -10250,31 +10497,31 @@
       <c r="V1" s="7"/>
     </row>
     <row r="2" spans="1:22" ht="204.75">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="23" t="s">
         <v>247</v>
       </c>
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="23" t="s">
         <v>248</v>
       </c>
-      <c r="D2" s="57" t="s">
+      <c r="D2" s="23" t="s">
         <v>249</v>
       </c>
-      <c r="E2" s="57" t="s">
+      <c r="E2" s="23" t="s">
         <v>250</v>
       </c>
-      <c r="F2" s="57" t="s">
+      <c r="F2" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="57" t="s">
+      <c r="G2" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="56" t="s">
+      <c r="H2" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="I2" s="58" t="s">
+      <c r="I2" s="49" t="s">
         <v>293</v>
       </c>
       <c r="J2" s="3"/>
@@ -10292,31 +10539,31 @@
       <c r="V2" s="3"/>
     </row>
     <row r="3" spans="1:22" ht="189">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="23" t="s">
         <v>251</v>
       </c>
-      <c r="C3" s="57" t="s">
+      <c r="C3" s="23" t="s">
         <v>248</v>
       </c>
-      <c r="D3" s="57" t="s">
+      <c r="D3" s="23" t="s">
         <v>252</v>
       </c>
-      <c r="E3" s="57" t="s">
+      <c r="E3" s="23" t="s">
         <v>253</v>
       </c>
-      <c r="F3" s="57" t="s">
+      <c r="F3" s="23" t="s">
         <v>219</v>
       </c>
-      <c r="G3" s="57" t="s">
+      <c r="G3" s="23" t="s">
         <v>219</v>
       </c>
-      <c r="H3" s="56" t="s">
+      <c r="H3" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="I3" s="58"/>
+      <c r="I3" s="49"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -10332,31 +10579,31 @@
       <c r="V3" s="3"/>
     </row>
     <row r="4" spans="1:22" ht="189">
-      <c r="A4" s="56" t="s">
+      <c r="A4" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="57" t="s">
+      <c r="B4" s="23" t="s">
         <v>254</v>
       </c>
-      <c r="C4" s="57" t="s">
+      <c r="C4" s="23" t="s">
         <v>248</v>
       </c>
-      <c r="D4" s="59" t="s">
+      <c r="D4" s="24" t="s">
         <v>252</v>
       </c>
-      <c r="E4" s="59" t="s">
+      <c r="E4" s="24" t="s">
         <v>255</v>
       </c>
-      <c r="F4" s="57" t="s">
+      <c r="F4" s="23" t="s">
         <v>219</v>
       </c>
-      <c r="G4" s="57" t="s">
+      <c r="G4" s="23" t="s">
         <v>219</v>
       </c>
-      <c r="H4" s="56" t="s">
+      <c r="H4" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="I4" s="58"/>
+      <c r="I4" s="49"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
@@ -10372,31 +10619,31 @@
       <c r="V4" s="3"/>
     </row>
     <row r="5" spans="1:22" ht="189">
-      <c r="A5" s="56" t="s">
+      <c r="A5" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="B5" s="57" t="s">
+      <c r="B5" s="23" t="s">
         <v>256</v>
       </c>
-      <c r="C5" s="57" t="s">
+      <c r="C5" s="23" t="s">
         <v>248</v>
       </c>
-      <c r="D5" s="57" t="s">
+      <c r="D5" s="23" t="s">
         <v>252</v>
       </c>
-      <c r="E5" s="57" t="s">
+      <c r="E5" s="23" t="s">
         <v>257</v>
       </c>
-      <c r="F5" s="57" t="s">
+      <c r="F5" s="23" t="s">
         <v>219</v>
       </c>
-      <c r="G5" s="57" t="s">
+      <c r="G5" s="23" t="s">
         <v>219</v>
       </c>
-      <c r="H5" s="56" t="s">
+      <c r="H5" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="I5" s="58"/>
+      <c r="I5" s="49"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
@@ -10412,31 +10659,31 @@
       <c r="V5" s="3"/>
     </row>
     <row r="6" spans="1:22" ht="189">
-      <c r="A6" s="56" t="s">
+      <c r="A6" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="B6" s="57" t="s">
+      <c r="B6" s="23" t="s">
         <v>254</v>
       </c>
-      <c r="C6" s="57" t="s">
+      <c r="C6" s="23" t="s">
         <v>248</v>
       </c>
-      <c r="D6" s="57" t="s">
+      <c r="D6" s="23" t="s">
         <v>252</v>
       </c>
-      <c r="E6" s="57" t="s">
+      <c r="E6" s="23" t="s">
         <v>255</v>
       </c>
-      <c r="F6" s="57" t="s">
+      <c r="F6" s="23" t="s">
         <v>219</v>
       </c>
-      <c r="G6" s="57" t="s">
+      <c r="G6" s="23" t="s">
         <v>219</v>
       </c>
-      <c r="H6" s="56" t="s">
+      <c r="H6" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="I6" s="58"/>
+      <c r="I6" s="49"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
@@ -10452,31 +10699,31 @@
       <c r="V6" s="3"/>
     </row>
     <row r="7" spans="1:22" ht="189">
-      <c r="A7" s="56" t="s">
+      <c r="A7" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="57" t="s">
+      <c r="B7" s="23" t="s">
         <v>258</v>
       </c>
-      <c r="C7" s="57" t="s">
+      <c r="C7" s="23" t="s">
         <v>248</v>
       </c>
-      <c r="D7" s="57" t="s">
+      <c r="D7" s="23" t="s">
         <v>252</v>
       </c>
-      <c r="E7" s="57" t="s">
+      <c r="E7" s="23" t="s">
         <v>259</v>
       </c>
-      <c r="F7" s="57" t="s">
+      <c r="F7" s="23" t="s">
         <v>260</v>
       </c>
-      <c r="G7" s="57" t="s">
+      <c r="G7" s="23" t="s">
         <v>260</v>
       </c>
-      <c r="H7" s="56" t="s">
+      <c r="H7" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="I7" s="58"/>
+      <c r="I7" s="49"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
@@ -10492,31 +10739,31 @@
       <c r="V7" s="3"/>
     </row>
     <row r="8" spans="1:22" ht="189">
-      <c r="A8" s="56" t="s">
+      <c r="A8" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="B8" s="57" t="s">
+      <c r="B8" s="23" t="s">
         <v>261</v>
       </c>
-      <c r="C8" s="57" t="s">
+      <c r="C8" s="23" t="s">
         <v>248</v>
       </c>
-      <c r="D8" s="57" t="s">
+      <c r="D8" s="23" t="s">
         <v>252</v>
       </c>
-      <c r="E8" s="57" t="s">
+      <c r="E8" s="23" t="s">
         <v>262</v>
       </c>
-      <c r="F8" s="57" t="s">
+      <c r="F8" s="23" t="s">
         <v>263</v>
       </c>
-      <c r="G8" s="57" t="s">
+      <c r="G8" s="23" t="s">
         <v>263</v>
       </c>
-      <c r="H8" s="56" t="s">
+      <c r="H8" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="I8" s="58"/>
+      <c r="I8" s="49"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
@@ -10532,31 +10779,31 @@
       <c r="V8" s="3"/>
     </row>
     <row r="9" spans="1:22" ht="189">
-      <c r="A9" s="56" t="s">
+      <c r="A9" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="B9" s="57" t="s">
+      <c r="B9" s="23" t="s">
         <v>264</v>
       </c>
-      <c r="C9" s="57" t="s">
+      <c r="C9" s="23" t="s">
         <v>248</v>
       </c>
-      <c r="D9" s="57" t="s">
+      <c r="D9" s="23" t="s">
         <v>252</v>
       </c>
-      <c r="E9" s="57" t="s">
+      <c r="E9" s="23" t="s">
         <v>265</v>
       </c>
-      <c r="F9" s="57" t="s">
+      <c r="F9" s="23" t="s">
         <v>266</v>
       </c>
-      <c r="G9" s="57" t="s">
+      <c r="G9" s="23" t="s">
         <v>266</v>
       </c>
-      <c r="H9" s="56" t="s">
+      <c r="H9" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="I9" s="58"/>
+      <c r="I9" s="49"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
@@ -10572,31 +10819,31 @@
       <c r="V9" s="3"/>
     </row>
     <row r="10" spans="1:22" ht="189">
-      <c r="A10" s="56" t="s">
+      <c r="A10" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="B10" s="57" t="s">
+      <c r="B10" s="23" t="s">
         <v>267</v>
       </c>
-      <c r="C10" s="57" t="s">
+      <c r="C10" s="23" t="s">
         <v>248</v>
       </c>
-      <c r="D10" s="57" t="s">
+      <c r="D10" s="23" t="s">
         <v>252</v>
       </c>
-      <c r="E10" s="57" t="s">
+      <c r="E10" s="23" t="s">
         <v>268</v>
       </c>
-      <c r="F10" s="57" t="s">
+      <c r="F10" s="23" t="s">
         <v>269</v>
       </c>
-      <c r="G10" s="57" t="s">
+      <c r="G10" s="23" t="s">
         <v>269</v>
       </c>
-      <c r="H10" s="56" t="s">
+      <c r="H10" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="I10" s="58"/>
+      <c r="I10" s="49"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
@@ -10612,31 +10859,31 @@
       <c r="V10" s="3"/>
     </row>
     <row r="11" spans="1:22" ht="189">
-      <c r="A11" s="56" t="s">
+      <c r="A11" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="B11" s="57" t="s">
+      <c r="B11" s="23" t="s">
         <v>270</v>
       </c>
-      <c r="C11" s="57" t="s">
+      <c r="C11" s="23" t="s">
         <v>248</v>
       </c>
-      <c r="D11" s="57" t="s">
+      <c r="D11" s="23" t="s">
         <v>252</v>
       </c>
-      <c r="E11" s="57" t="s">
+      <c r="E11" s="23" t="s">
         <v>271</v>
       </c>
-      <c r="F11" s="57" t="s">
+      <c r="F11" s="23" t="s">
         <v>272</v>
       </c>
-      <c r="G11" s="57" t="s">
+      <c r="G11" s="23" t="s">
         <v>272</v>
       </c>
-      <c r="H11" s="56" t="s">
+      <c r="H11" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="I11" s="58"/>
+      <c r="I11" s="49"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
@@ -10652,31 +10899,31 @@
       <c r="V11" s="3"/>
     </row>
     <row r="12" spans="1:22" ht="110.25">
-      <c r="A12" s="56" t="s">
+      <c r="A12" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="B12" s="57" t="s">
+      <c r="B12" s="23" t="s">
         <v>273</v>
       </c>
-      <c r="C12" s="57" t="s">
+      <c r="C12" s="23" t="s">
         <v>248</v>
       </c>
-      <c r="D12" s="57" t="s">
+      <c r="D12" s="23" t="s">
         <v>274</v>
       </c>
-      <c r="E12" s="57" t="s">
+      <c r="E12" s="23" t="s">
         <v>275</v>
       </c>
-      <c r="F12" s="57" t="s">
+      <c r="F12" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="57" t="s">
+      <c r="G12" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="H12" s="56" t="s">
+      <c r="H12" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="I12" s="58"/>
+      <c r="I12" s="49"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
@@ -10692,29 +10939,29 @@
       <c r="V12" s="3"/>
     </row>
     <row r="13" spans="1:22" ht="63">
-      <c r="A13" s="56" t="s">
+      <c r="A13" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="B13" s="57" t="s">
+      <c r="B13" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="57" t="s">
+      <c r="C13" s="23" t="s">
         <v>248</v>
       </c>
-      <c r="D13" s="57" t="s">
+      <c r="D13" s="23" t="s">
         <v>276</v>
       </c>
-      <c r="E13" s="57"/>
-      <c r="F13" s="57" t="s">
+      <c r="E13" s="23"/>
+      <c r="F13" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="G13" s="57" t="s">
+      <c r="G13" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="H13" s="56" t="s">
+      <c r="H13" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="I13" s="58"/>
+      <c r="I13" s="49"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
@@ -10730,29 +10977,29 @@
       <c r="V13" s="3"/>
     </row>
     <row r="14" spans="1:22" ht="63">
-      <c r="A14" s="56" t="s">
+      <c r="A14" s="22" t="s">
         <v>242</v>
       </c>
-      <c r="B14" s="57" t="s">
+      <c r="B14" s="23" t="s">
         <v>245</v>
       </c>
-      <c r="C14" s="57" t="s">
+      <c r="C14" s="23" t="s">
         <v>248</v>
       </c>
-      <c r="D14" s="57" t="s">
+      <c r="D14" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="E14" s="57"/>
-      <c r="F14" s="57" t="s">
+      <c r="E14" s="23"/>
+      <c r="F14" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="G14" s="57" t="s">
+      <c r="G14" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="H14" s="56" t="s">
+      <c r="H14" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="I14" s="58"/>
+      <c r="I14" s="49"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
@@ -12118,7 +12365,7 @@
     <col min="23" max="16384" width="14.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="8" customFormat="1">
+    <row r="1" spans="1:22" s="8" customFormat="1" ht="25.5">
       <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
@@ -12161,31 +12408,31 @@
       <c r="V1" s="7"/>
     </row>
     <row r="2" spans="1:22" ht="126">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="23" t="s">
         <v>207</v>
       </c>
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="23" t="s">
         <v>208</v>
       </c>
-      <c r="D2" s="57" t="s">
+      <c r="D2" s="23" t="s">
         <v>209</v>
       </c>
-      <c r="E2" s="57" t="s">
+      <c r="E2" s="23" t="s">
         <v>210</v>
       </c>
-      <c r="F2" s="57" t="s">
+      <c r="F2" s="23" t="s">
         <v>211</v>
       </c>
-      <c r="G2" s="57" t="s">
+      <c r="G2" s="23" t="s">
         <v>211</v>
       </c>
-      <c r="H2" s="75" t="s">
+      <c r="H2" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="58" t="s">
+      <c r="I2" s="49" t="s">
         <v>293</v>
       </c>
       <c r="J2" s="3"/>
@@ -12203,31 +12450,31 @@
       <c r="V2" s="3"/>
     </row>
     <row r="3" spans="1:22" ht="126">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="23" t="s">
         <v>212</v>
       </c>
-      <c r="C3" s="57" t="s">
+      <c r="C3" s="23" t="s">
         <v>208</v>
       </c>
-      <c r="D3" s="57" t="s">
+      <c r="D3" s="23" t="s">
         <v>209</v>
       </c>
-      <c r="E3" s="57" t="s">
+      <c r="E3" s="23" t="s">
         <v>213</v>
       </c>
-      <c r="F3" s="57" t="s">
+      <c r="F3" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="57" t="s">
+      <c r="G3" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="75" t="s">
+      <c r="H3" s="34" t="s">
         <v>121</v>
       </c>
-      <c r="I3" s="58"/>
+      <c r="I3" s="49"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -12243,31 +12490,31 @@
       <c r="V3" s="3"/>
     </row>
     <row r="4" spans="1:22" ht="126">
-      <c r="A4" s="56" t="s">
+      <c r="A4" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="57" t="s">
+      <c r="B4" s="23" t="s">
         <v>214</v>
       </c>
-      <c r="C4" s="57" t="s">
+      <c r="C4" s="23" t="s">
         <v>208</v>
       </c>
-      <c r="D4" s="57" t="s">
+      <c r="D4" s="23" t="s">
         <v>209</v>
       </c>
-      <c r="E4" s="57" t="s">
+      <c r="E4" s="23" t="s">
         <v>215</v>
       </c>
-      <c r="F4" s="57" t="s">
+      <c r="F4" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="57" t="s">
+      <c r="G4" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="75" t="s">
+      <c r="H4" s="34" t="s">
         <v>121</v>
       </c>
-      <c r="I4" s="58"/>
+      <c r="I4" s="49"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
@@ -12283,31 +12530,31 @@
       <c r="V4" s="3"/>
     </row>
     <row r="5" spans="1:22" ht="110.25">
-      <c r="A5" s="56" t="s">
+      <c r="A5" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="B5" s="57" t="s">
+      <c r="B5" s="23" t="s">
         <v>216</v>
       </c>
-      <c r="C5" s="57" t="s">
+      <c r="C5" s="23" t="s">
         <v>208</v>
       </c>
-      <c r="D5" s="57" t="s">
+      <c r="D5" s="23" t="s">
         <v>217</v>
       </c>
-      <c r="E5" s="57" t="s">
+      <c r="E5" s="23" t="s">
         <v>218</v>
       </c>
-      <c r="F5" s="57" t="s">
+      <c r="F5" s="23" t="s">
         <v>219</v>
       </c>
-      <c r="G5" s="57" t="s">
+      <c r="G5" s="23" t="s">
         <v>219</v>
       </c>
-      <c r="H5" s="75" t="s">
+      <c r="H5" s="34" t="s">
         <v>121</v>
       </c>
-      <c r="I5" s="58"/>
+      <c r="I5" s="49"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
@@ -12323,31 +12570,31 @@
       <c r="V5" s="3"/>
     </row>
     <row r="6" spans="1:22" ht="110.25">
-      <c r="A6" s="56" t="s">
+      <c r="A6" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="B6" s="57" t="s">
+      <c r="B6" s="23" t="s">
         <v>220</v>
       </c>
-      <c r="C6" s="57" t="s">
+      <c r="C6" s="23" t="s">
         <v>208</v>
       </c>
-      <c r="D6" s="57" t="s">
+      <c r="D6" s="23" t="s">
         <v>217</v>
       </c>
-      <c r="E6" s="57" t="s">
+      <c r="E6" s="23" t="s">
         <v>221</v>
       </c>
-      <c r="F6" s="57" t="s">
+      <c r="F6" s="23" t="s">
         <v>219</v>
       </c>
-      <c r="G6" s="57" t="s">
+      <c r="G6" s="23" t="s">
         <v>219</v>
       </c>
-      <c r="H6" s="75" t="s">
+      <c r="H6" s="34" t="s">
         <v>121</v>
       </c>
-      <c r="I6" s="58"/>
+      <c r="I6" s="49"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
@@ -12363,31 +12610,31 @@
       <c r="V6" s="3"/>
     </row>
     <row r="7" spans="1:22" ht="110.25">
-      <c r="A7" s="56" t="s">
+      <c r="A7" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="57" t="s">
+      <c r="B7" s="23" t="s">
         <v>222</v>
       </c>
-      <c r="C7" s="57" t="s">
+      <c r="C7" s="23" t="s">
         <v>208</v>
       </c>
-      <c r="D7" s="57" t="s">
+      <c r="D7" s="23" t="s">
         <v>217</v>
       </c>
-      <c r="E7" s="57" t="s">
+      <c r="E7" s="23" t="s">
         <v>223</v>
       </c>
-      <c r="F7" s="57" t="s">
+      <c r="F7" s="23" t="s">
         <v>219</v>
       </c>
-      <c r="G7" s="57" t="s">
+      <c r="G7" s="23" t="s">
         <v>219</v>
       </c>
-      <c r="H7" s="75" t="s">
+      <c r="H7" s="34" t="s">
         <v>121</v>
       </c>
-      <c r="I7" s="58"/>
+      <c r="I7" s="49"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
@@ -12403,31 +12650,31 @@
       <c r="V7" s="3"/>
     </row>
     <row r="8" spans="1:22" ht="110.25">
-      <c r="A8" s="56" t="s">
+      <c r="A8" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="B8" s="57" t="s">
+      <c r="B8" s="23" t="s">
         <v>224</v>
       </c>
-      <c r="C8" s="57" t="s">
+      <c r="C8" s="23" t="s">
         <v>208</v>
       </c>
-      <c r="D8" s="57" t="s">
+      <c r="D8" s="23" t="s">
         <v>217</v>
       </c>
-      <c r="E8" s="57" t="s">
+      <c r="E8" s="23" t="s">
         <v>225</v>
       </c>
-      <c r="F8" s="57" t="s">
+      <c r="F8" s="23" t="s">
         <v>226</v>
       </c>
-      <c r="G8" s="57" t="s">
+      <c r="G8" s="23" t="s">
         <v>226</v>
       </c>
-      <c r="H8" s="75" t="s">
+      <c r="H8" s="34" t="s">
         <v>121</v>
       </c>
-      <c r="I8" s="58"/>
+      <c r="I8" s="49"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
@@ -12443,31 +12690,31 @@
       <c r="V8" s="3"/>
     </row>
     <row r="9" spans="1:22" ht="110.25">
-      <c r="A9" s="56" t="s">
+      <c r="A9" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="B9" s="57" t="s">
+      <c r="B9" s="23" t="s">
         <v>227</v>
       </c>
-      <c r="C9" s="57" t="s">
+      <c r="C9" s="23" t="s">
         <v>208</v>
       </c>
-      <c r="D9" s="57" t="s">
+      <c r="D9" s="23" t="s">
         <v>217</v>
       </c>
-      <c r="E9" s="57" t="s">
+      <c r="E9" s="23" t="s">
         <v>228</v>
       </c>
-      <c r="F9" s="57" t="s">
+      <c r="F9" s="23" t="s">
         <v>229</v>
       </c>
-      <c r="G9" s="57" t="s">
+      <c r="G9" s="23" t="s">
         <v>229</v>
       </c>
-      <c r="H9" s="75" t="s">
+      <c r="H9" s="34" t="s">
         <v>121</v>
       </c>
-      <c r="I9" s="58"/>
+      <c r="I9" s="49"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
@@ -12483,31 +12730,31 @@
       <c r="V9" s="3"/>
     </row>
     <row r="10" spans="1:22" ht="110.25">
-      <c r="A10" s="56" t="s">
+      <c r="A10" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="B10" s="57" t="s">
+      <c r="B10" s="23" t="s">
         <v>230</v>
       </c>
-      <c r="C10" s="57" t="s">
+      <c r="C10" s="23" t="s">
         <v>208</v>
       </c>
-      <c r="D10" s="57" t="s">
+      <c r="D10" s="23" t="s">
         <v>217</v>
       </c>
-      <c r="E10" s="57" t="s">
+      <c r="E10" s="23" t="s">
         <v>231</v>
       </c>
-      <c r="F10" s="57" t="s">
+      <c r="F10" s="23" t="s">
         <v>232</v>
       </c>
-      <c r="G10" s="57" t="s">
+      <c r="G10" s="23" t="s">
         <v>232</v>
       </c>
-      <c r="H10" s="75" t="s">
+      <c r="H10" s="34" t="s">
         <v>121</v>
       </c>
-      <c r="I10" s="58"/>
+      <c r="I10" s="49"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
@@ -12523,31 +12770,31 @@
       <c r="V10" s="3"/>
     </row>
     <row r="11" spans="1:22" ht="110.25">
-      <c r="A11" s="56" t="s">
+      <c r="A11" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="B11" s="57" t="s">
+      <c r="B11" s="23" t="s">
         <v>233</v>
       </c>
-      <c r="C11" s="57" t="s">
+      <c r="C11" s="23" t="s">
         <v>208</v>
       </c>
-      <c r="D11" s="57" t="s">
+      <c r="D11" s="23" t="s">
         <v>217</v>
       </c>
-      <c r="E11" s="57" t="s">
+      <c r="E11" s="23" t="s">
         <v>234</v>
       </c>
-      <c r="F11" s="57" t="s">
+      <c r="F11" s="23" t="s">
         <v>235</v>
       </c>
-      <c r="G11" s="57" t="s">
+      <c r="G11" s="23" t="s">
         <v>235</v>
       </c>
-      <c r="H11" s="75" t="s">
+      <c r="H11" s="34" t="s">
         <v>121</v>
       </c>
-      <c r="I11" s="58"/>
+      <c r="I11" s="49"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
@@ -12563,31 +12810,31 @@
       <c r="V11" s="3"/>
     </row>
     <row r="12" spans="1:22" ht="126">
-      <c r="A12" s="56" t="s">
+      <c r="A12" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="B12" s="57" t="s">
+      <c r="B12" s="23" t="s">
         <v>236</v>
       </c>
-      <c r="C12" s="57" t="s">
+      <c r="C12" s="23" t="s">
         <v>208</v>
       </c>
-      <c r="D12" s="57" t="s">
+      <c r="D12" s="23" t="s">
         <v>209</v>
       </c>
-      <c r="E12" s="57" t="s">
+      <c r="E12" s="23" t="s">
         <v>237</v>
       </c>
-      <c r="F12" s="57" t="s">
+      <c r="F12" s="23" t="s">
         <v>238</v>
       </c>
-      <c r="G12" s="57" t="s">
+      <c r="G12" s="23" t="s">
         <v>238</v>
       </c>
-      <c r="H12" s="75" t="s">
+      <c r="H12" s="34" t="s">
         <v>121</v>
       </c>
-      <c r="I12" s="58"/>
+      <c r="I12" s="49"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
@@ -12603,31 +12850,31 @@
       <c r="V12" s="3"/>
     </row>
     <row r="13" spans="1:22" ht="78.75">
-      <c r="A13" s="56" t="s">
+      <c r="A13" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="B13" s="57" t="s">
+      <c r="B13" s="23" t="s">
         <v>239</v>
       </c>
-      <c r="C13" s="57" t="s">
+      <c r="C13" s="23" t="s">
         <v>208</v>
       </c>
-      <c r="D13" s="57" t="s">
+      <c r="D13" s="23" t="s">
         <v>240</v>
       </c>
-      <c r="E13" s="57" t="s">
+      <c r="E13" s="23" t="s">
         <v>241</v>
       </c>
-      <c r="F13" s="57" t="s">
+      <c r="F13" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="57" t="s">
+      <c r="G13" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="H13" s="75" t="s">
+      <c r="H13" s="34" t="s">
         <v>121</v>
       </c>
-      <c r="I13" s="58"/>
+      <c r="I13" s="49"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
@@ -12643,29 +12890,29 @@
       <c r="V13" s="3"/>
     </row>
     <row r="14" spans="1:22" ht="63">
-      <c r="A14" s="56" t="s">
+      <c r="A14" s="22" t="s">
         <v>242</v>
       </c>
-      <c r="B14" s="57" t="s">
+      <c r="B14" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="57" t="s">
+      <c r="C14" s="23" t="s">
         <v>208</v>
       </c>
-      <c r="D14" s="57" t="s">
+      <c r="D14" s="23" t="s">
         <v>243</v>
       </c>
-      <c r="E14" s="57"/>
-      <c r="F14" s="57" t="s">
+      <c r="E14" s="23"/>
+      <c r="F14" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="57" t="s">
+      <c r="G14" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="H14" s="75" t="s">
+      <c r="H14" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="I14" s="58"/>
+      <c r="I14" s="49"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
@@ -12681,29 +12928,29 @@
       <c r="V14" s="3"/>
     </row>
     <row r="15" spans="1:22" ht="63">
-      <c r="A15" s="56" t="s">
+      <c r="A15" s="22" t="s">
         <v>244</v>
       </c>
-      <c r="B15" s="57" t="s">
+      <c r="B15" s="23" t="s">
         <v>245</v>
       </c>
-      <c r="C15" s="57" t="s">
+      <c r="C15" s="23" t="s">
         <v>208</v>
       </c>
-      <c r="D15" s="57" t="s">
+      <c r="D15" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="E15" s="57"/>
-      <c r="F15" s="57" t="s">
+      <c r="E15" s="23"/>
+      <c r="F15" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="G15" s="57" t="s">
+      <c r="G15" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="H15" s="75" t="s">
+      <c r="H15" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="I15" s="58"/>
+      <c r="I15" s="49"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>

</xml_diff>